<commit_message>
Task List updated for 'Attendance report for specified period'-(US-4)
</commit_message>
<xml_diff>
--- a/Klipper US.xlsx
+++ b/Klipper US.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4170"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4170" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="US List" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="79">
   <si>
     <t>User Stories</t>
   </si>
@@ -312,6 +312,15 @@
   </si>
   <si>
     <t>4th</t>
+  </si>
+  <si>
+    <t>Show user's data for selected date range: API</t>
+  </si>
+  <si>
+    <t>Show user's data for selected date range: UI</t>
+  </si>
+  <si>
+    <t>Repository implementation</t>
   </si>
 </sst>
 </file>
@@ -841,7 +850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -1692,8 +1701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1734,25 +1743,55 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>

</xml_diff>

<commit_message>
Updated tasks for Usecase: Show list of reportees
</commit_message>
<xml_diff>
--- a/Klipper US.xlsx
+++ b/Klipper US.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4170"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4170" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="US List" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="77">
   <si>
     <t>User Stories</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>Siddhesh</t>
-  </si>
-  <si>
-    <t>Naushad</t>
   </si>
   <si>
     <t>For Only Valid input
@@ -249,12 +246,6 @@
     <t>Remaining Time(hrs)</t>
   </si>
   <si>
-    <t>Show selected user's data : API</t>
-  </si>
-  <si>
-    <t>Show selected user's data : UI</t>
-  </si>
-  <si>
     <t>Dummy password for users</t>
   </si>
   <si>
@@ -275,9 +266,6 @@
     <t>Highlight deficiate data</t>
   </si>
   <si>
-    <t>completed</t>
-  </si>
-  <si>
     <t>Issues</t>
   </si>
   <si>
@@ -302,16 +290,31 @@
     <t>US1</t>
   </si>
   <si>
-    <t>Visibilities of reportees : UI</t>
-  </si>
-  <si>
-    <t>List of reportees : API</t>
-  </si>
-  <si>
     <t xml:space="preserve">3rd </t>
   </si>
   <si>
     <t>4th</t>
+  </si>
+  <si>
+    <t>Identify roles</t>
+  </si>
+  <si>
+    <t>Get list of reportees for individual Admin/Lead</t>
+  </si>
+  <si>
+    <t>If role is Admin/Lead, then show list of reportees</t>
+  </si>
+  <si>
+    <t>On selection of reportee, show one week Attendance record</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Check whether usecase is running with all scenarios</t>
+  </si>
+  <si>
+    <t>To do</t>
   </si>
 </sst>
 </file>
@@ -841,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,7 +866,7 @@
     </row>
     <row r="2" spans="2:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2"/>
       <c r="F2"/>
@@ -875,7 +878,7 @@
     </row>
     <row r="5" spans="2:7" s="12" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>0</v>
@@ -887,10 +890,10 @@
         <v>10</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -910,7 +913,7 @@
         <v>43448</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -928,7 +931,7 @@
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
@@ -955,13 +958,13 @@
         <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -973,13 +976,13 @@
         <v>6</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -991,13 +994,13 @@
         <v>7</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -1006,16 +1009,16 @@
         <v>6</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G13" s="1"/>
     </row>
@@ -1024,10 +1027,10 @@
         <v>7</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>2</v>
@@ -1036,7 +1039,7 @@
         <v>43452</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1112,10 +1115,10 @@
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B2" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
@@ -1123,19 +1126,19 @@
     </row>
     <row r="4" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B4" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="22" t="s">
+      <c r="E4" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="15" t="s">
         <v>25</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -1143,16 +1146,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -1160,16 +1163,16 @@
         <v>2</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -1177,16 +1180,16 @@
         <v>3</v>
       </c>
       <c r="C7" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="E7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -1194,16 +1197,16 @@
         <v>4</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -1211,16 +1214,16 @@
         <v>5</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -1228,16 +1231,16 @@
         <v>6</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -1321,10 +1324,10 @@
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B2" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>32</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>33</v>
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
@@ -1332,19 +1335,19 @@
     </row>
     <row r="4" spans="2:6" s="16" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -1352,7 +1355,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="23">
         <v>3</v>
@@ -1361,7 +1364,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -1369,16 +1372,16 @@
         <v>2</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -1386,7 +1389,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D7" s="1">
         <v>2</v>
@@ -1395,7 +1398,7 @@
         <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -1403,16 +1406,16 @@
         <v>4</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D8" s="1">
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -1492,16 +1495,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F18"/>
+  <dimension ref="B2:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46" customWidth="1"/>
+    <col min="3" max="3" width="56" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" style="2" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
@@ -1509,10 +1512,10 @@
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B2" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
@@ -1520,19 +1523,19 @@
     </row>
     <row r="4" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B4" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="22" t="s">
+      <c r="E4" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="15" t="s">
         <v>25</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -1540,16 +1543,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D5" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -1557,16 +1560,14 @@
         <v>2</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" s="1">
-        <v>4</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -1574,16 +1575,16 @@
         <v>3</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="D7" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -1591,16 +1592,16 @@
         <v>4</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="D8" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -1608,7 +1609,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="D9" s="1">
         <v>3</v>
@@ -1617,7 +1618,7 @@
         <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -1647,41 +1648,6 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1707,10 +1673,10 @@
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B2" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>36</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>37</v>
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
@@ -1718,19 +1684,19 @@
     </row>
     <row r="4" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B4" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="22" t="s">
+      <c r="E4" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="15" t="s">
         <v>25</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -1855,10 +1821,10 @@
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B2" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="28" t="s">
         <v>38</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>39</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="21"/>
@@ -1866,19 +1832,19 @@
     </row>
     <row r="4" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B4" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="22" t="s">
+      <c r="E4" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="15" t="s">
         <v>25</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -2006,10 +1972,10 @@
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B2" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>30</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>31</v>
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
@@ -2017,19 +1983,19 @@
     </row>
     <row r="4" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B4" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="22" t="s">
+      <c r="E4" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="15" t="s">
         <v>25</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -2156,27 +2122,27 @@
     <row r="2" spans="3:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C2" s="20"/>
       <c r="D2" s="17" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="3:8" ht="51.75" x14ac:dyDescent="0.25">
       <c r="C4" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="22" t="s">
+      <c r="F4" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>26</v>
-      </c>
       <c r="H4" s="15" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.25">
@@ -2184,19 +2150,19 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="H5" s="13" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
@@ -2204,19 +2170,19 @@
         <v>2</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="H6" s="13" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
@@ -2224,19 +2190,19 @@
         <v>3</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="H7" s="13" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
@@ -2244,19 +2210,19 @@
         <v>4</v>
       </c>
       <c r="D8" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="13" t="s">
         <v>67</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
@@ -2264,19 +2230,19 @@
         <v>5</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
user story 6 task define
</commit_message>
<xml_diff>
--- a/Klipper US.xlsx
+++ b/Klipper US.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4170" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4170" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="US List" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="83">
   <si>
     <t>User Stories</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Siddhesh</t>
+  </si>
+  <si>
+    <t>Naushad</t>
   </si>
   <si>
     <t>For Only Valid input
@@ -246,6 +249,12 @@
     <t>Remaining Time(hrs)</t>
   </si>
   <si>
+    <t>Show selected user's data : API</t>
+  </si>
+  <si>
+    <t>Show selected user's data : UI</t>
+  </si>
+  <si>
     <t>Dummy password for users</t>
   </si>
   <si>
@@ -266,6 +275,9 @@
     <t>Highlight deficiate data</t>
   </si>
   <si>
+    <t>completed</t>
+  </si>
+  <si>
     <t>Issues</t>
   </si>
   <si>
@@ -290,31 +302,37 @@
     <t>US1</t>
   </si>
   <si>
+    <t>Visibilities of reportees : UI</t>
+  </si>
+  <si>
+    <t>List of reportees : API</t>
+  </si>
+  <si>
     <t xml:space="preserve">3rd </t>
   </si>
   <si>
     <t>4th</t>
   </si>
   <si>
-    <t>Identify roles</t>
-  </si>
-  <si>
-    <t>Get list of reportees for individual Admin/Lead</t>
-  </si>
-  <si>
-    <t>If role is Admin/Lead, then show list of reportees</t>
-  </si>
-  <si>
-    <t>On selection of reportee, show one week Attendance record</t>
-  </si>
-  <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>Check whether usecase is running with all scenarios</t>
-  </si>
-  <si>
-    <t>To do</t>
+    <t>Show user's data for selected date range: API</t>
+  </si>
+  <si>
+    <t>Show user's data for selected date range: UI</t>
+  </si>
+  <si>
+    <t>Repository implementation</t>
+  </si>
+  <si>
+    <t>To Do</t>
+  </si>
+  <si>
+    <t>Get list of detail of access event of a day.</t>
+  </si>
+  <si>
+    <t>Display popup of detail access event on UI .</t>
+  </si>
+  <si>
+    <t>Design Popup for display access event .</t>
   </si>
 </sst>
 </file>
@@ -844,8 +862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,7 +884,7 @@
     </row>
     <row r="2" spans="2:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2"/>
       <c r="F2"/>
@@ -878,7 +896,7 @@
     </row>
     <row r="5" spans="2:7" s="12" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>0</v>
@@ -890,10 +908,10 @@
         <v>10</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -913,7 +931,7 @@
         <v>43448</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -931,7 +949,7 @@
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
@@ -958,13 +976,13 @@
         <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -976,13 +994,13 @@
         <v>6</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -994,13 +1012,13 @@
         <v>7</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -1009,16 +1027,16 @@
         <v>6</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="G13" s="1"/>
     </row>
@@ -1027,10 +1045,10 @@
         <v>7</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>2</v>
@@ -1039,7 +1057,7 @@
         <v>43452</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1115,10 +1133,10 @@
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B2" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>28</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>27</v>
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
@@ -1126,19 +1144,19 @@
     </row>
     <row r="4" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B4" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>22</v>
-      </c>
       <c r="D4" s="22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E4" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="15" t="s">
         <v>26</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -1146,16 +1164,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -1163,16 +1181,16 @@
         <v>2</v>
       </c>
       <c r="C6" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -1180,16 +1198,16 @@
         <v>3</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -1197,16 +1215,16 @@
         <v>4</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -1214,16 +1232,16 @@
         <v>5</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -1231,16 +1249,16 @@
         <v>6</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -1324,10 +1342,10 @@
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B2" s="20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
@@ -1335,19 +1353,19 @@
     </row>
     <row r="4" spans="2:6" s="16" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>22</v>
-      </c>
       <c r="D4" s="22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E4" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="15" t="s">
         <v>26</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -1355,7 +1373,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D5" s="23">
         <v>3</v>
@@ -1364,7 +1382,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -1372,16 +1390,16 @@
         <v>2</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -1389,7 +1407,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D7" s="1">
         <v>2</v>
@@ -1398,7 +1416,7 @@
         <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -1406,16 +1424,16 @@
         <v>4</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D8" s="1">
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -1495,171 +1513,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B2" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-    </row>
-    <row r="4" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B4" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="1">
-        <v>2</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="1">
-        <v>3</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" s="1">
-        <v>3</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="1">
-        <v>4</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" s="1">
-        <v>3</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="1">
-        <v>5</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D9" s="1">
-        <v>3</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1676,7 +1533,7 @@
         <v>35</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
@@ -1684,41 +1541,269 @@
     </row>
     <row r="4" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B4" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>23</v>
       </c>
+      <c r="D4" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="1">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>4</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>5</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B2" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+    </row>
+    <row r="4" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B4" s="15" t="s">
+        <v>24</v>
+      </c>
       <c r="C4" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E4" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
@@ -1821,10 +1906,10 @@
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B2" s="20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="21"/>
@@ -1832,19 +1917,19 @@
     </row>
     <row r="4" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B4" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>22</v>
-      </c>
       <c r="D4" s="22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E4" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="15" t="s">
         <v>26</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -1957,8 +2042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1972,10 +2057,10 @@
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B2" s="20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
@@ -1983,41 +2068,71 @@
     </row>
     <row r="4" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B4" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>22</v>
-      </c>
       <c r="D4" s="22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E4" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="1">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="1">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="1">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
@@ -2122,27 +2237,27 @@
     <row r="2" spans="3:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C2" s="20"/>
       <c r="D2" s="17" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="3:8" ht="51.75" x14ac:dyDescent="0.25">
       <c r="C4" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>22</v>
-      </c>
       <c r="E4" s="22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F4" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="15" t="s">
-        <v>25</v>
-      </c>
       <c r="H4" s="15" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.25">
@@ -2150,19 +2265,19 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
@@ -2170,19 +2285,19 @@
         <v>2</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
@@ -2190,19 +2305,19 @@
         <v>3</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
@@ -2210,19 +2325,19 @@
         <v>4</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
@@ -2230,19 +2345,19 @@
         <v>5</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the task for User story 5
</commit_message>
<xml_diff>
--- a/Klipper US.xlsx
+++ b/Klipper US.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4170" activeTab="6"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="14352" windowHeight="4176" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="US List" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="89">
   <si>
     <t>User Stories</t>
   </si>
@@ -308,21 +308,12 @@
     <t>List of reportees : API</t>
   </si>
   <si>
-    <t xml:space="preserve">3rd </t>
-  </si>
-  <si>
-    <t>4th</t>
-  </si>
-  <si>
     <t>Show user's data for selected date range: API</t>
   </si>
   <si>
     <t>Show user's data for selected date range: UI</t>
   </si>
   <si>
-    <t>Repository implementation</t>
-  </si>
-  <si>
     <t>To Do</t>
   </si>
   <si>
@@ -333,6 +324,35 @@
   </si>
   <si>
     <t>Design Popup for display access event .</t>
+  </si>
+  <si>
+    <t>Export Report as csv,PDF</t>
+  </si>
+  <si>
+    <t>Write test cases</t>
+  </si>
+  <si>
+    <t>Get the data from Repository</t>
+  </si>
+  <si>
+    <t>9th</t>
+  </si>
+  <si>
+    <t>10th</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deficit hrs calculation according to policy document. 
+Total Deficit Hrs, Total Overtime Hrs
+</t>
+  </si>
+  <si>
+    <t>Show Total hrs for the selected data</t>
+  </si>
+  <si>
+    <t>Export options for Attendance Report</t>
+  </si>
+  <si>
+    <t>To do</t>
   </si>
 </sst>
 </file>
@@ -860,24 +880,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G22"/>
+  <dimension ref="B1:G21"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" customWidth="1"/>
     <col min="2" max="2" width="12" style="2" customWidth="1"/>
-    <col min="3" max="3" width="44.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="39.140625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="39.109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="C1"/>
       <c r="D1"/>
       <c r="F1"/>
@@ -889,7 +909,7 @@
       <c r="D2"/>
       <c r="F2"/>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="C3"/>
       <c r="D3"/>
       <c r="F3"/>
@@ -952,7 +972,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="3"/>
       <c r="D8" s="5"/>
@@ -960,7 +980,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="3"/>
       <c r="D9" s="5"/>
@@ -982,7 +1002,7 @@
         <v>11</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -1000,7 +1020,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -1018,7 +1038,7 @@
         <v>13</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -1036,7 +1056,7 @@
         <v>12</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G13" s="1"/>
     </row>
@@ -1053,52 +1073,67 @@
       <c r="E14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="27">
-        <v>43452</v>
-      </c>
+      <c r="F14" s="27"/>
       <c r="G14" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="F15"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="F16"/>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>8</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="2:7" s="4" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>9</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="3:6" ht="15" x14ac:dyDescent="0.25">
       <c r="C17"/>
       <c r="D17"/>
       <c r="F17"/>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:6" ht="15" x14ac:dyDescent="0.25">
       <c r="C18"/>
       <c r="D18"/>
       <c r="F18"/>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:6" ht="15" x14ac:dyDescent="0.25">
       <c r="C19"/>
       <c r="D19"/>
       <c r="F19"/>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:6" ht="15" x14ac:dyDescent="0.25">
       <c r="C20"/>
       <c r="D20"/>
       <c r="F20"/>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:6" ht="15" x14ac:dyDescent="0.25">
       <c r="C21"/>
       <c r="D21"/>
       <c r="F21"/>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="F22"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -1122,13 +1157,13 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
@@ -1159,7 +1194,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -1176,7 +1211,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -1193,7 +1228,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -1210,7 +1245,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>4</v>
       </c>
@@ -1227,7 +1262,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>5</v>
       </c>
@@ -1244,7 +1279,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>6</v>
       </c>
@@ -1261,56 +1296,56 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="13"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="13"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="13"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="13"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="13"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="13"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="13"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="13"/>
       <c r="D18" s="1"/>
@@ -1331,13 +1366,13 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
@@ -1368,7 +1403,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -1385,7 +1420,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -1402,7 +1437,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -1419,7 +1454,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>4</v>
       </c>
@@ -1436,70 +1471,70 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="13"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="13"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="13"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="13"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="13"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="13"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="13"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="13"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="13"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="13"/>
       <c r="D18" s="1"/>
@@ -1516,16 +1551,16 @@
   <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
@@ -1556,7 +1591,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -1573,7 +1608,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -1590,7 +1625,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -1607,7 +1642,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>4</v>
       </c>
@@ -1624,7 +1659,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>5</v>
       </c>
@@ -1641,63 +1676,71 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-      <c r="C10" s="13"/>
+    <row r="10" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>6</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>81</v>
+      </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="13"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="13"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="13"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="13"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="13"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="13"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="13"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="13"/>
       <c r="D18" s="1"/>
@@ -1714,16 +1757,16 @@
   <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B6" sqref="B6:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
@@ -1754,12 +1797,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D5" s="1">
         <v>2</v>
@@ -1768,15 +1811,15 @@
         <v>2</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D6" s="1">
         <v>2</v>
@@ -1785,15 +1828,15 @@
         <v>2</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
@@ -1802,80 +1845,88 @@
         <v>2</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>4</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="13"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="13"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="13"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="13"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="13"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="13"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="13"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="13"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="13"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="13"/>
       <c r="D18" s="1"/>
@@ -1891,17 +1942,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
@@ -1932,98 +1983,128 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="13"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="13"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="13"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="13"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="13"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="13"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="13"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="13"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="13"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="13"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="13"/>
       <c r="D18" s="1"/>
@@ -2042,17 +2123,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
@@ -2083,12 +2164,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D5" s="1">
         <v>6</v>
@@ -2097,15 +2178,15 @@
         <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D6" s="1">
         <v>5</v>
@@ -2114,15 +2195,15 @@
         <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D7" s="1">
         <v>8</v>
@@ -2131,80 +2212,80 @@
         <v>12</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="13"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="13"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="13"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="13"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="13"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="13"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="13"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="13"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="13"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="13"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="13"/>
       <c r="D18" s="1"/>
@@ -2224,14 +2305,14 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:8" ht="17.25" x14ac:dyDescent="0.3">
@@ -2260,7 +2341,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:8" ht="15" x14ac:dyDescent="0.25">
       <c r="C5" s="1">
         <v>1</v>
       </c>
@@ -2280,7 +2361,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:8" ht="15" x14ac:dyDescent="0.25">
       <c r="C6" s="1">
         <v>2</v>
       </c>
@@ -2300,7 +2381,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:8" ht="15" x14ac:dyDescent="0.25">
       <c r="C7" s="1">
         <v>3</v>
       </c>
@@ -2320,7 +2401,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:8" ht="15" x14ac:dyDescent="0.25">
       <c r="C8" s="1">
         <v>4</v>
       </c>
@@ -2340,7 +2421,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:8" ht="15" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
updated tasks status for user story 3
</commit_message>
<xml_diff>
--- a/Klipper US.xlsx
+++ b/Klipper US.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="14352" windowHeight="4176" activeTab="6"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4170" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="US List" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="89">
   <si>
     <t>User Stories</t>
   </si>
@@ -350,6 +350,9 @@
   </si>
   <si>
     <t>Visibility of Reportee tab for lead and admin</t>
+  </si>
+  <si>
+    <t>Merging</t>
   </si>
 </sst>
 </file>
@@ -880,21 +883,21 @@
   <dimension ref="B1:G21"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
     <col min="2" max="2" width="12" style="2" customWidth="1"/>
-    <col min="3" max="3" width="44.6640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="39.109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="44.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="39.140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C1"/>
       <c r="D1"/>
       <c r="F1"/>
@@ -906,7 +909,7 @@
       <c r="D2"/>
       <c r="F2"/>
     </row>
-    <row r="3" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C3"/>
       <c r="D3"/>
       <c r="F3"/>
@@ -969,7 +972,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="3"/>
       <c r="D8" s="5"/>
@@ -977,7 +980,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="2:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="3"/>
       <c r="D9" s="5"/>
@@ -1107,27 +1110,27 @@
       <c r="F16" s="3"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="3:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17"/>
       <c r="D17"/>
       <c r="F17"/>
     </row>
-    <row r="18" spans="3:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18"/>
       <c r="D18"/>
       <c r="F18"/>
     </row>
-    <row r="19" spans="3:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19"/>
       <c r="D19"/>
       <c r="F19"/>
     </row>
-    <row r="20" spans="3:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20"/>
       <c r="D20"/>
       <c r="F20"/>
     </row>
-    <row r="21" spans="3:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C21"/>
       <c r="D21"/>
       <c r="F21"/>
@@ -1154,13 +1157,13 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
@@ -1191,7 +1194,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -1208,7 +1211,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -1225,7 +1228,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -1242,7 +1245,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>4</v>
       </c>
@@ -1259,7 +1262,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>5</v>
       </c>
@@ -1276,7 +1279,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>6</v>
       </c>
@@ -1293,56 +1296,56 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="13"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="13"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="13"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="13"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="13"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="13"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="13"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="13"/>
       <c r="D18" s="1"/>
@@ -1363,13 +1366,13 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="25.109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
@@ -1400,7 +1403,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -1417,7 +1420,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -1434,7 +1437,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -1451,7 +1454,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>4</v>
       </c>
@@ -1468,70 +1471,70 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="13"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="13"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="13"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="13"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="13"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="13"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="13"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="13"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="13"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="13"/>
       <c r="D18" s="1"/>
@@ -1547,17 +1550,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
@@ -1588,7 +1591,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -1605,7 +1608,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -1622,7 +1625,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -1633,18 +1636,18 @@
         <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>4</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="D8" s="1">
         <v>3</v>
@@ -1656,77 +1659,83 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>5</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1">
+        <v>3</v>
+      </c>
       <c r="E9" s="1" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>6</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="D10" s="1">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="F10" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="13"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="13"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="13"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="13"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="13"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="13"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="13"/>
       <c r="D17" s="1"/>
@@ -1746,13 +1755,13 @@
       <selection activeCell="B6" sqref="B6:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
@@ -1783,7 +1792,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -1800,7 +1809,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -1817,7 +1826,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -1834,7 +1843,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>4</v>
       </c>
@@ -1849,70 +1858,70 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="13"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="13"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="13"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="13"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="13"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="13"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="13"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="13"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="13"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="13"/>
       <c r="D18" s="1"/>
@@ -1932,13 +1941,13 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
@@ -1969,7 +1978,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -1986,7 +1995,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -2003,7 +2012,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -2020,77 +2029,77 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="13"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="13"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="13"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="13"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="13"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="13"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="13"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="13"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="13"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="13"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="13"/>
       <c r="D18" s="1"/>
@@ -2109,17 +2118,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
@@ -2150,7 +2159,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -2167,7 +2176,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -2184,7 +2193,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -2201,77 +2210,77 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="13"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="13"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="13"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="13"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="13"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="13"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="13"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="13"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="13"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="13"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="13"/>
       <c r="D18" s="1"/>
@@ -2291,14 +2300,14 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:8" ht="17.25" x14ac:dyDescent="0.3">
@@ -2327,7 +2336,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="3:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C5" s="1">
         <v>1</v>
       </c>
@@ -2347,7 +2356,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="3:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C6" s="1">
         <v>2</v>
       </c>
@@ -2367,7 +2376,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="3:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" s="1">
         <v>3</v>
       </c>
@@ -2387,7 +2396,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="3:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C8" s="1">
         <v>4</v>
       </c>
@@ -2407,7 +2416,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="3:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Updated US 7 in Klipper excel file
</commit_message>
<xml_diff>
--- a/Klipper US.xlsx
+++ b/Klipper US.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4170" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4170" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="US List" sheetId="1" r:id="rId1"/>
@@ -14,15 +14,15 @@
     <sheet name="US 4" sheetId="5" r:id="rId5"/>
     <sheet name="US 5" sheetId="6" r:id="rId6"/>
     <sheet name="US 6" sheetId="7" r:id="rId7"/>
-    <sheet name="Issues" sheetId="8" r:id="rId8"/>
+    <sheet name="US7" sheetId="9" r:id="rId8"/>
+    <sheet name="Issues" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="104">
   <si>
     <t>User Stories</t>
   </si>
@@ -350,17 +350,88 @@
     <t>To do</t>
   </si>
   <si>
-    <t>Visibility of Reportee tab for lead and admin</t>
-  </si>
-  <si>
-    <t>Merging</t>
+    <t>US 7</t>
+  </si>
+  <si>
+    <t>Server Environment setup</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>InProgress</t>
+  </si>
+  <si>
+    <r>
+      <t>Server Environment setup-</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ProductionMachine</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>server accessible within network-</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ProductionMachine</t>
+    </r>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Change in script(Read data for last 2 days only)</t>
+  </si>
+  <si>
+    <t>Deploy data-sync-schedular script on server</t>
+  </si>
+  <si>
+    <t>Change in script(sync extra fields from Access to Mongo)</t>
+  </si>
+  <si>
+    <t>Make script available on github</t>
+  </si>
+  <si>
+    <t>Add logging mechanism to script</t>
+  </si>
+  <si>
+    <t>Data comparison and monitoring for a week</t>
+  </si>
+  <si>
+    <t>Visibilit of reportee tab for lead and admin only</t>
+  </si>
+  <si>
+    <t>SIdhdesh</t>
+  </si>
+  <si>
+    <t>Add test cases</t>
+  </si>
+  <si>
+    <t>Test cases</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -402,6 +473,14 @@
     </font>
     <font>
       <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -883,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,7 +1234,7 @@
   <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1298,11 +1377,21 @@
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="B11" s="1">
+        <v>7</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
@@ -1412,7 +1501,7 @@
         <v>49</v>
       </c>
       <c r="D5" s="23">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E5" s="24" t="s">
         <v>12</v>
@@ -1446,7 +1535,7 @@
         <v>60</v>
       </c>
       <c r="D7" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>11</v>
@@ -1463,7 +1552,7 @@
         <v>51</v>
       </c>
       <c r="D8" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>52</v>
@@ -1473,11 +1562,21 @@
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="B9" s="1">
+        <v>5</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
@@ -1551,8 +1650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1600,7 +1699,7 @@
         <v>70</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>42</v>
@@ -1617,7 +1716,7 @@
         <v>71</v>
       </c>
       <c r="D6" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>42</v>
@@ -1634,7 +1733,7 @@
         <v>54</v>
       </c>
       <c r="D7" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>42</v>
@@ -1648,13 +1747,13 @@
         <v>4</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>88</v>
+        <v>51</v>
       </c>
       <c r="D8" s="1">
         <v>3</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>11</v>
+        <v>101</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>41</v>
@@ -1682,7 +1781,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
@@ -1753,7 +1852,7 @@
   <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1937,7 +2036,7 @@
   <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2021,9 +2120,7 @@
       <c r="D7" s="1">
         <v>3</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
         <v>86</v>
       </c>
@@ -2118,7 +2215,7 @@
   <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2292,6 +2389,233 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:F19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B3" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="2:6" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>4</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>5</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>6</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>7</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <v>8</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>9</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:H9"/>
   <sheetViews>
@@ -2437,6 +2761,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
some changes on controller for displaying data for provided dates
</commit_message>
<xml_diff>
--- a/Klipper US.xlsx
+++ b/Klipper US.xlsx
@@ -18,6 +18,7 @@
     <sheet name="Issues" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -2036,7 +2037,7 @@
   <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2076,7 +2077,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -2087,13 +2088,13 @@
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Update tasks progress on klipper excel
</commit_message>
<xml_diff>
--- a/Klipper US.xlsx
+++ b/Klipper US.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4170" activeTab="5"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="14352" windowHeight="4176" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="US List" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,11 @@
     <sheet name="Issues" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="104">
   <si>
     <t>User Stories</t>
   </si>
@@ -967,18 +966,18 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" customWidth="1"/>
     <col min="2" max="2" width="12" style="2" customWidth="1"/>
-    <col min="3" max="3" width="44.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="39.140625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="39.109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="C1"/>
       <c r="D1"/>
       <c r="F1"/>
@@ -990,7 +989,7 @@
       <c r="D2"/>
       <c r="F2"/>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="C3"/>
       <c r="D3"/>
       <c r="F3"/>
@@ -1053,7 +1052,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="3"/>
       <c r="D8" s="5"/>
@@ -1061,7 +1060,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="3"/>
       <c r="D9" s="5"/>
@@ -1191,27 +1190,27 @@
       <c r="F16" s="3"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:6" ht="15" x14ac:dyDescent="0.25">
       <c r="C17"/>
       <c r="D17"/>
       <c r="F17"/>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:6" ht="15" x14ac:dyDescent="0.25">
       <c r="C18"/>
       <c r="D18"/>
       <c r="F18"/>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:6" ht="15" x14ac:dyDescent="0.25">
       <c r="C19"/>
       <c r="D19"/>
       <c r="F19"/>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:6" ht="15" x14ac:dyDescent="0.25">
       <c r="C20"/>
       <c r="D20"/>
       <c r="F20"/>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:6" ht="15" x14ac:dyDescent="0.25">
       <c r="C21"/>
       <c r="D21"/>
       <c r="F21"/>
@@ -1238,13 +1237,13 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
@@ -1275,7 +1274,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -1292,7 +1291,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -1309,7 +1308,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -1326,7 +1325,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>4</v>
       </c>
@@ -1343,7 +1342,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>5</v>
       </c>
@@ -1360,7 +1359,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>6</v>
       </c>
@@ -1377,7 +1376,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>7</v>
       </c>
@@ -1394,49 +1393,49 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="13"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="13"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="13"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="13"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="13"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="13"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="13"/>
       <c r="D18" s="1"/>
@@ -1457,13 +1456,13 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
@@ -1494,7 +1493,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -1511,7 +1510,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -1528,7 +1527,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -1545,7 +1544,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>4</v>
       </c>
@@ -1562,7 +1561,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>5</v>
       </c>
@@ -1579,63 +1578,63 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="13"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="13"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="13"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="13"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="13"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="13"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="13"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="13"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="13"/>
       <c r="D18" s="1"/>
@@ -1652,16 +1651,16 @@
   <dimension ref="B2:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
@@ -1692,7 +1691,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -1709,7 +1708,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -1726,7 +1725,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -1743,7 +1742,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>4</v>
       </c>
@@ -1757,10 +1756,10 @@
         <v>101</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>5</v>
       </c>
@@ -1777,7 +1776,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>6</v>
       </c>
@@ -1794,49 +1793,49 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="13"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="13"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="13"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="13"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="13"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="13"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="13"/>
       <c r="D17" s="1"/>
@@ -1856,13 +1855,13 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
@@ -1893,7 +1892,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -1910,7 +1909,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -1927,7 +1926,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -1944,7 +1943,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>4</v>
       </c>
@@ -1957,70 +1956,70 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="13"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="13"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="13"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="13"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="13"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="13"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="13"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="13"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="13"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="13"/>
       <c r="D18" s="1"/>
@@ -2034,19 +2033,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F18"/>
+  <dimension ref="B2:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
@@ -2077,7 +2076,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -2085,7 +2084,7 @@
         <v>73</v>
       </c>
       <c r="D5" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>42</v>
@@ -2094,114 +2093,97 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>2</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="1">
-        <v>3</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="D7" s="1">
-        <v>3</v>
-      </c>
+    <row r="7" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="13"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="13"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="13"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="13"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="13"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="13"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="13"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="13"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="13"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="13"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2219,13 +2201,13 @@
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
@@ -2256,7 +2238,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -2273,7 +2255,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -2290,7 +2272,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -2307,77 +2289,77 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="13"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="13"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="13"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="13"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="13"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="13"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="13"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="13"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="13"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="13"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="13"/>
       <c r="D18" s="1"/>
@@ -2393,17 +2375,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -2417,7 +2399,7 @@
       <c r="E3" s="21"/>
       <c r="F3" s="21"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -2440,7 +2422,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>1</v>
       </c>
@@ -2455,7 +2437,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>2</v>
       </c>
@@ -2470,7 +2452,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>3</v>
       </c>
@@ -2485,7 +2467,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>4</v>
       </c>
@@ -2500,7 +2482,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>5</v>
       </c>
@@ -2515,7 +2497,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>6</v>
       </c>
@@ -2530,7 +2512,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>7</v>
       </c>
@@ -2545,7 +2527,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>8</v>
       </c>
@@ -2560,7 +2542,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>9</v>
       </c>
@@ -2575,35 +2557,35 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="13"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="13"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="13"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="13"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="13"/>
       <c r="D19" s="1"/>
@@ -2624,14 +2606,14 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:8" ht="17.25" x14ac:dyDescent="0.3">
@@ -2660,7 +2642,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:8" ht="15" x14ac:dyDescent="0.25">
       <c r="C5" s="1">
         <v>1</v>
       </c>
@@ -2680,7 +2662,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:8" ht="15" x14ac:dyDescent="0.25">
       <c r="C6" s="1">
         <v>2</v>
       </c>
@@ -2700,7 +2682,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:8" ht="15" x14ac:dyDescent="0.25">
       <c r="C7" s="1">
         <v>3</v>
       </c>
@@ -2720,7 +2702,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:8" ht="15" x14ac:dyDescent="0.25">
       <c r="C8" s="1">
         <v>4</v>
       </c>
@@ -2740,7 +2722,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:8" ht="15" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Updated the tasks for user story 8
</commit_message>
<xml_diff>
--- a/Klipper US.xlsx
+++ b/Klipper US.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="14352" windowHeight="4176" activeTab="5"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4170" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="US List" sheetId="1" r:id="rId1"/>
@@ -14,15 +14,16 @@
     <sheet name="US 4" sheetId="5" r:id="rId5"/>
     <sheet name="US 5" sheetId="6" r:id="rId6"/>
     <sheet name="US 6" sheetId="7" r:id="rId7"/>
-    <sheet name="US7" sheetId="9" r:id="rId8"/>
-    <sheet name="Issues" sheetId="8" r:id="rId9"/>
+    <sheet name="US7 " sheetId="12" r:id="rId8"/>
+    <sheet name="US8" sheetId="9" r:id="rId9"/>
+    <sheet name="Issues" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="108">
   <si>
     <t>User Stories</t>
   </si>
@@ -425,6 +426,18 @@
   </si>
   <si>
     <t>Test cases</t>
+  </si>
+  <si>
+    <t>Calculate Total working hours and total deficit/overtime hours for specified date range</t>
+  </si>
+  <si>
+    <t>write test cases</t>
+  </si>
+  <si>
+    <t>US 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UI - show total working hours and deficit/overtime hours </t>
   </si>
 </sst>
 </file>
@@ -963,21 +976,21 @@
   <dimension ref="B1:G21"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:H11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
     <col min="2" max="2" width="12" style="2" customWidth="1"/>
-    <col min="3" max="3" width="44.6640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="39.109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="44.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="39.140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C1"/>
       <c r="D1"/>
       <c r="F1"/>
@@ -989,7 +1002,7 @@
       <c r="D2"/>
       <c r="F2"/>
     </row>
-    <row r="3" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C3"/>
       <c r="D3"/>
       <c r="F3"/>
@@ -1052,7 +1065,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="3"/>
       <c r="D8" s="5"/>
@@ -1060,7 +1073,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="2:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="3"/>
       <c r="D9" s="5"/>
@@ -1196,27 +1209,27 @@
       <c r="F16" s="3"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="3:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17"/>
       <c r="D17"/>
       <c r="F17"/>
     </row>
-    <row r="18" spans="3:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18"/>
       <c r="D18"/>
       <c r="F18"/>
     </row>
-    <row r="19" spans="3:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19"/>
       <c r="D19"/>
       <c r="F19"/>
     </row>
-    <row r="20" spans="3:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20"/>
       <c r="D20"/>
       <c r="F20"/>
     </row>
-    <row r="21" spans="3:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C21"/>
       <c r="D21"/>
       <c r="F21"/>
@@ -1235,6 +1248,156 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="C2" s="20"/>
+      <c r="D2" s="17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="3:8" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="C4" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="1">
+        <v>3</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="1">
+        <v>5</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F18"/>
@@ -1243,13 +1406,13 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
@@ -1280,7 +1443,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -1297,7 +1460,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -1314,7 +1477,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -1331,7 +1494,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>4</v>
       </c>
@@ -1348,7 +1511,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>5</v>
       </c>
@@ -1365,7 +1528,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>6</v>
       </c>
@@ -1382,7 +1545,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>7</v>
       </c>
@@ -1399,49 +1562,49 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="13"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="13"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="13"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="13"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="13"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="13"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="13"/>
       <c r="D18" s="1"/>
@@ -1462,13 +1625,13 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="25.109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
@@ -1499,7 +1662,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -1516,7 +1679,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -1533,7 +1696,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -1550,7 +1713,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>4</v>
       </c>
@@ -1567,7 +1730,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>5</v>
       </c>
@@ -1584,63 +1747,63 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="13"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="13"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="13"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="13"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="13"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="13"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="13"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="13"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="13"/>
       <c r="D18" s="1"/>
@@ -1660,13 +1823,13 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
@@ -1697,7 +1860,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -1714,7 +1877,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -1731,7 +1894,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -1748,7 +1911,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>4</v>
       </c>
@@ -1765,7 +1928,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>5</v>
       </c>
@@ -1782,7 +1945,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>6</v>
       </c>
@@ -1799,49 +1962,49 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="13"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="13"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="13"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="13"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="13"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="13"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="13"/>
       <c r="D17" s="1"/>
@@ -1861,13 +2024,13 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
@@ -1898,7 +2061,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -1915,7 +2078,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -1932,7 +2095,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -1949,7 +2112,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>4</v>
       </c>
@@ -1962,70 +2125,70 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="13"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="13"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="13"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="13"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="13"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="13"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="13"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="13"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="13"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="13"/>
       <c r="D18" s="1"/>
@@ -2041,17 +2204,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
@@ -2082,7 +2245,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -2099,7 +2262,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>3</v>
       </c>
@@ -2114,77 +2277,77 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="13"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="13"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="13"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="13"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="13"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="13"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="13"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="13"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="13"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="13"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="13"/>
       <c r="D17" s="1"/>
@@ -2204,16 +2367,16 @@
   <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" s="16" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
@@ -2244,7 +2407,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -2261,7 +2424,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -2278,7 +2441,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -2295,77 +2458,77 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="13"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="13"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="13"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="13"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="13"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="13"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="13"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="13"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="13"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="13"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="13"/>
       <c r="D18" s="1"/>
@@ -2382,16 +2545,16 @@
   <dimension ref="B3:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -2405,7 +2568,7 @@
       <c r="E3" s="21"/>
       <c r="F3" s="21"/>
     </row>
-    <row r="4" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -2428,7 +2591,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>1</v>
       </c>
@@ -2443,7 +2606,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>2</v>
       </c>
@@ -2458,7 +2621,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>3</v>
       </c>
@@ -2473,7 +2636,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>4</v>
       </c>
@@ -2488,7 +2651,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>5</v>
       </c>
@@ -2503,7 +2666,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>6</v>
       </c>
@@ -2518,7 +2681,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>7</v>
       </c>
@@ -2533,7 +2696,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>8</v>
       </c>
@@ -2548,7 +2711,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>9</v>
       </c>
@@ -2563,35 +2726,35 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="13"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="13"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="13"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="13"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="13"/>
       <c r="D19" s="1"/>
@@ -2606,150 +2769,108 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:H9"/>
+  <dimension ref="B3:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="79.140625" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C2" s="20"/>
-      <c r="D2" s="17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="3:8" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="C4" s="15" t="s">
+    <row r="3" spans="2:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B3" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="2:6" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="C5" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="D5" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="E5" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="F5" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="3:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="C5" s="1">
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="3:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="C6" s="1">
-        <v>2</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>63</v>
+      <c r="C6" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>48</v>
+        <v>2</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="3:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="C7" s="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
         <v>3</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="3:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="C8" s="1">
-        <v>4</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>65</v>
+      <c r="C8" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="3:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="C9" s="1">
-        <v>5</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes in User story task update
</commit_message>
<xml_diff>
--- a/Klipper US.xlsx
+++ b/Klipper US.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanket\Downloads\Compressed\NewKlipper-Departmentwise_working_days_and_hours\NewKlipper-Departmentwise_working_days_and_hours\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A072A1-48CA-408C-9BC1-E2D178FC569B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4170" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4170" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="US List" sheetId="1" r:id="rId1"/>
@@ -32,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="118">
   <si>
     <t>User Stories</t>
   </si>
@@ -449,11 +443,14 @@
   <si>
     <t>lead can cancel realised leave</t>
   </si>
+  <si>
+    <t>5hrs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -665,9 +662,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -689,6 +683,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -725,7 +722,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -784,7 +781,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -817,26 +814,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -869,23 +849,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1061,7 +1024,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G21"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -1117,189 +1080,189 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="22">
+      <c r="B6" s="21">
         <v>1</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="24">
         <v>43448</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="21" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="22">
+      <c r="B7" s="21">
         <v>2</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22" t="s">
+      <c r="F7" s="21"/>
+      <c r="G7" s="21" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="8" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="22"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="22"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" spans="2:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="22">
+      <c r="B10" s="21">
         <v>3</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="G10" s="22"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="2:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="22">
+      <c r="B11" s="21">
         <v>4</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="G11" s="22"/>
+      <c r="G11" s="21"/>
     </row>
     <row r="12" spans="2:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="22">
+      <c r="B12" s="21">
         <v>5</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="G12" s="22"/>
+      <c r="G12" s="21"/>
     </row>
     <row r="13" spans="2:7" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="22">
+      <c r="B13" s="21">
         <v>6</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="G13" s="22"/>
+      <c r="G13" s="21"/>
     </row>
     <row r="14" spans="2:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="22">
+      <c r="B14" s="21">
         <v>7</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="D14" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="25"/>
-      <c r="G14" s="22" t="s">
+      <c r="F14" s="24"/>
+      <c r="G14" s="21" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="22">
+      <c r="B15" s="21">
         <v>8</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="27"/>
-      <c r="G15" s="22"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="21"/>
     </row>
     <row r="16" spans="2:7" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="22">
+      <c r="B16" s="21">
         <v>9</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="D16" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="E16" s="22" t="s">
+      <c r="E16" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F16" s="26"/>
-      <c r="G16" s="22"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="21"/>
     </row>
     <row r="17" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <v>10</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="28" t="s">
         <v>90</v>
       </c>
       <c r="F17"/>
@@ -1326,10 +1289,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G14" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G14">
       <formula1>"Open,In-Progress,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6">
       <formula1>"Open,In-Progress,Completed,Closed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1339,7 +1302,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60FBDBC8-8506-43AF-BC59-5BDB816EF185}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1537,7 +1500,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{815A8FBC-1BF3-4D4B-982F-83B094A97589}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1723,7 +1686,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88D84581-EBEB-4EAE-B2C1-C2BF9C5EA13B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1909,7 +1872,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2059,7 +2022,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2268,7 +2231,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -2456,7 +2419,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2662,7 +2625,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2848,7 +2811,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2868,10 +2831,10 @@
       <c r="B2" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="21"/>
+      <c r="D2" s="29"/>
       <c r="E2" s="17"/>
       <c r="F2" s="17"/>
     </row>
@@ -3029,7 +2992,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3207,11 +3170,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F74EAA1-868B-40CF-AE08-871459DA377B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3310,9 +3273,11 @@
         <v>92</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="F8" s="1" t="s">
-        <v>88</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -3365,10 +3330,12 @@
       <c r="C12" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
@@ -3436,7 +3403,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF9970E9-DAF5-49C7-BC9F-FCE798142940}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>